<commit_message>
ajustes finais para entrega
</commit_message>
<xml_diff>
--- a/ps4.xlsx
+++ b/ps4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a92579583e6a5f9b/Desktop/Insper/Ciência de Dados/Projeto-1-CDados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Insper\2° Semestre\Ciência dos Dados\Projeto 1 CDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="114_{59723F87-05B1-40CC-B51D-7E9F88220C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADD46A8C-8075-477C-83B9-0FBDC07FA30C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C489C57E-BA08-4836-B63B-27D026CA08BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1867,7 +1867,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1884,7 +1884,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2206,17 +2206,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B302"/>
   <sheetViews>
-    <sheetView topLeftCell="A282" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A302" sqref="A302"/>
+    <sheetView topLeftCell="A285" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B302" sqref="B302"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="206.6328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" customWidth="1"/>
+    <col min="1" max="1" width="206.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>65</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>87</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>115</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>120</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>122</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>123</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>124</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>126</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>127</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>130</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>131</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>133</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>134</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>136</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>137</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>139</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>140</v>
       </c>
@@ -3344,12 +3344,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>142</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>143</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>144</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>145</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>146</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>147</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>148</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>152</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>153</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>154</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>155</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>156</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>157</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>158</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>159</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>160</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>161</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>162</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>163</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>164</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>165</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>166</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>167</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>168</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>169</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>170</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>171</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>172</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>173</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>174</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>175</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>176</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>177</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>178</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>179</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>180</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>181</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>182</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>183</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>184</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>185</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>186</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>187</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>188</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>189</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>190</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>191</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>192</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>193</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>194</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>195</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>196</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>197</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>198</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>199</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>200</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>201</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>202</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>203</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>204</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>205</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>206</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>207</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>208</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>209</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>210</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>211</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>212</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>213</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>214</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>215</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>216</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>217</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>218</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>219</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>220</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>221</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>222</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>223</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>224</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>225</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>226</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>227</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>228</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>229</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>230</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>231</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>232</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>233</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>234</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>235</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>236</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>237</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>238</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>239</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>240</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>241</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>242</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>243</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>244</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>245</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>246</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>247</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>248</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>249</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>250</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>251</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>252</v>
       </c>
@@ -4237,12 +4237,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>254</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>255</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
         <v>256</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>257</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>258</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>259</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>260</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
         <v>261</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>262</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>263</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
         <v>264</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>265</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
         <v>266</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
         <v>267</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
         <v>268</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
         <v>269</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
         <v>270</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
         <v>271</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
         <v>272</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
         <v>273</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
         <v>274</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
         <v>275</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
         <v>276</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
         <v>277</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" s="2" t="s">
         <v>278</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A280" s="2" t="s">
         <v>279</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" s="2" t="s">
         <v>280</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" s="2" t="s">
         <v>281</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" s="2" t="s">
         <v>282</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A284" s="2" t="s">
         <v>283</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A285" s="2" t="s">
         <v>284</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
         <v>285</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" s="2" t="s">
         <v>286</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" s="2" t="s">
         <v>287</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
         <v>288</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
         <v>289</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
         <v>290</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
         <v>291</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A293" s="2" t="s">
         <v>292</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" s="2" t="s">
         <v>293</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
         <v>294</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" s="2" t="s">
         <v>295</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" s="2" t="s">
         <v>296</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
         <v>297</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
         <v>298</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
         <v>299</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
         <v>300</v>
       </c>
@@ -4618,9 +4618,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B302">
-        <f>SUM(B2:B284)</f>
+        <f>SUM(B2:B282)</f>
         <v>123</v>
       </c>
     </row>
@@ -4635,19 +4635,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="206" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>302</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>303</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>304</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>305</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>306</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>307</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>308</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>309</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>310</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>311</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>312</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>313</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>314</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>315</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>316</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>317</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>318</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>319</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>320</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>321</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>322</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>323</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>324</v>
       </c>
@@ -4839,23 +4839,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>325</v>
       </c>
       <c r="B25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>326</v>
       </c>
       <c r="B26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>327</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>328</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>329</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>330</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>331</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>332</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>333</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>334</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>335</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>336</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>337</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>338</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>339</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>340</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>341</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>342</v>
       </c>
@@ -4983,15 +4983,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>343</v>
       </c>
       <c r="B43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>344</v>
       </c>
@@ -4999,15 +4999,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>345</v>
       </c>
       <c r="B45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>346</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>347</v>
       </c>
@@ -5023,15 +5023,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>348</v>
       </c>
       <c r="B48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>349</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>350</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>351</v>
       </c>
@@ -5055,15 +5055,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>352</v>
       </c>
       <c r="B52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>353</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>354</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>355</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>356</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>357</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>358</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>359</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>360</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>361</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>362</v>
       </c>
@@ -5143,15 +5143,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>363</v>
       </c>
       <c r="B63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>364</v>
       </c>
@@ -5159,15 +5159,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>365</v>
       </c>
       <c r="B65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>366</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>367</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>368</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>369</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>370</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>371</v>
       </c>
@@ -5215,15 +5215,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>372</v>
       </c>
       <c r="B72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>373</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>374</v>
       </c>
@@ -5239,31 +5239,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>375</v>
       </c>
       <c r="B75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>376</v>
       </c>
       <c r="B76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>377</v>
       </c>
       <c r="B77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>378</v>
       </c>
@@ -5271,7 +5271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>379</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>380</v>
       </c>
@@ -5287,15 +5287,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>381</v>
       </c>
       <c r="B81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>382</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>383</v>
       </c>
@@ -5311,15 +5311,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>384</v>
       </c>
       <c r="B84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>385</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>386</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>387</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>388</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>389</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>390</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>391</v>
       </c>
@@ -5375,15 +5375,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>392</v>
       </c>
       <c r="B92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>393</v>
       </c>
@@ -5391,23 +5391,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>394</v>
       </c>
       <c r="B94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>395</v>
       </c>
       <c r="B95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>396</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>397</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>398</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>399</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>400</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>401</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>402</v>
       </c>
@@ -5463,15 +5463,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>403</v>
       </c>
       <c r="B103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>404</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>405</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>406</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>407</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>408</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>409</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>410</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>411</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>412</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>413</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>414</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>415</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>416</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>417</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>418</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>419</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>420</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>421</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>422</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>423</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>424</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>425</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>426</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>427</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>428</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>429</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>430</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>431</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>432</v>
       </c>
@@ -5703,7 +5703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>433</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>434</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>435</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>436</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>437</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>438</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>439</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>440</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>441</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>442</v>
       </c>
@@ -5783,7 +5783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>443</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>444</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>445</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>446</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>447</v>
       </c>
@@ -5823,15 +5823,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>448</v>
       </c>
       <c r="B148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>449</v>
       </c>
@@ -5839,7 +5839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>450</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>451</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>452</v>
       </c>
@@ -5863,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>453</v>
       </c>
@@ -5871,15 +5871,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>454</v>
       </c>
       <c r="B154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>455</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>456</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>457</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>458</v>
       </c>
@@ -5911,23 +5911,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>459</v>
       </c>
       <c r="B159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>460</v>
       </c>
       <c r="B160">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>461</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>462</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>463</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>464</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>465</v>
       </c>
@@ -5967,7 +5967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>466</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>467</v>
       </c>
@@ -5983,15 +5983,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>468</v>
       </c>
       <c r="B168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>469</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>470</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>471</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>472</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>473</v>
       </c>
@@ -6031,15 +6031,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>474</v>
       </c>
       <c r="B174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>475</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>476</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>477</v>
       </c>
@@ -6063,15 +6063,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>478</v>
       </c>
       <c r="B178">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>479</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>480</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>481</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>482</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>483</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>484</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>485</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>486</v>
       </c>
@@ -6135,7 +6135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>487</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>488</v>
       </c>
@@ -6151,7 +6151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>489</v>
       </c>
@@ -6159,15 +6159,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>490</v>
       </c>
       <c r="B190">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>491</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>492</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>493</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>494</v>
       </c>
@@ -6199,7 +6199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>495</v>
       </c>
@@ -6207,15 +6207,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>496</v>
       </c>
       <c r="B196">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>497</v>
       </c>
@@ -6223,7 +6223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>498</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>499</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>500</v>
       </c>
@@ -6247,12 +6247,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>501</v>
       </c>
       <c r="B201">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1048576">
+        <f>SUM(B2:B1048575)</f>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>